<commit_message>
af, mf, ss, ps
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH2.xlsx
@@ -85,7 +85,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>Moral Judgement (MJ) \n Ingroup/Outgroup (IO) \n Value of Life (VOL) \n Quality of Life (QOL)</t>
+    <t>AF, MF, SS, PS</t>
   </si>
   <si>
     <t xml:space="preserve">0.0-1.0 </t>
@@ -471,7 +471,7 @@
   <cols>
     <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="43.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="82.86214285714286" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="69.7192857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="36.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="28.719285714285714" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
Observation ADMs in RQ2.2-2.3 Table (#308)
* observation sets

* def
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH2.xlsx
@@ -64,7 +64,7 @@
     <t>Trials within set within attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Which random set of probes this adm was assigned. </t>
+    <t xml:space="preserve">If the set was dynamically generated or an observation set.  </t>
   </si>
   <si>
     <t>The session id used to get the alignment value of the aligned ADM at the specified target from the TA1 server</t>
@@ -85,7 +85,7 @@
     <t>0.0-1.0 OR 0.0_0.0  to 1.0_1.0 (Multi KDMA)</t>
   </si>
   <si>
-    <t>1-100</t>
+    <t>P2June Dynamic Set 1-100 / P2June Observation Set 1-3</t>
   </si>
   <si>
     <t>Individual or Group</t>
@@ -461,7 +461,7 @@
     <col min="2" max="2" style="2" width="43.14785714285715" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="82.86214285714286" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="69.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="36.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="47.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="28.719285714285714" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="43.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="96.14785714285713" customWidth="1" bestFit="1"/>
@@ -775,7 +775,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -787,7 +787,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -799,7 +799,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -811,7 +811,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -823,7 +823,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -835,7 +835,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -847,7 +847,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -859,7 +859,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>

</xml_diff>